<commit_message>
roller lever and float level switch
added prices for these switches
</commit_message>
<xml_diff>
--- a/List of Bills .xlsx
+++ b/List of Bills .xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Bill of materials </t>
   </si>
@@ -92,18 +92,22 @@
     <t>ip65</t>
   </si>
   <si>
-    <t xml:space="preserve">$23.46 each </t>
-  </si>
-  <si>
     <t xml:space="preserve">Slide door sensor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">float level switch </t>
+  </si>
+  <si>
+    <t>limit switch ,roller lever</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -142,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -154,7 +158,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:H15"/>
+  <dimension ref="C1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,19 +611,41 @@
       <c r="F14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G14" t="s">
-        <v>22</v>
+      <c r="G14" s="7">
+        <v>93.94</v>
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="7">
+        <v>18.29</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5">
-        <v>150</v>
+      <c r="E17" s="5">
+        <v>1</v>
+      </c>
+      <c r="G17" s="7">
+        <v>17.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>